<commit_message>
Corrected a few bugs and cleaned the code a bit
</commit_message>
<xml_diff>
--- a/Standards_concentrations.xlsx
+++ b/Standards_concentrations.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maverdier\Desktop\Programmation\Python\Volatils_GUI\volatils_GUI_v2.0\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Limage\Desktop\volatils_GUI_v2-0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EACDDF9-2311-4E4E-84CB-1DF985A7974A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="13200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17625"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>NAME</t>
   </si>
@@ -93,14 +92,23 @@
     <t>STR09</t>
   </si>
   <si>
-    <t>NS1</t>
+    <t>B</t>
+  </si>
+  <si>
+    <t>DL</t>
+  </si>
+  <si>
+    <t>LGB1</t>
+  </si>
+  <si>
+    <t>SCO</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -111,6 +119,17 @@
     <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -142,7 +161,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -150,6 +169,20 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="11" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -464,19 +497,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="12" width="11.3828125" style="1"/>
+    <col min="2" max="12" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -514,7 +547,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -531,7 +564,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -548,7 +581,7 @@
         <v>71.900000000000006</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -565,7 +598,7 @@
         <v>50.2</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -582,7 +615,7 @@
         <v>50.2</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -600,7 +633,7 @@
         <v>50.2</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -617,7 +650,7 @@
         <v>50.2</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -637,7 +670,7 @@
         <v>70.2</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -660,7 +693,7 @@
         <v>50.6</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -680,7 +713,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>17</v>
       </c>
@@ -688,15 +721,84 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>22</v>
       </c>
       <c r="B12" s="1">
-        <v>3150</v>
+        <v>0</v>
+      </c>
+      <c r="D12" s="1">
+        <v>0</v>
+      </c>
+      <c r="H12" s="1">
+        <v>0</v>
+      </c>
+      <c r="J12" s="1">
+        <v>0</v>
       </c>
       <c r="L12" s="1">
-        <v>49.4</v>
+        <v>78</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="5">
+        <v>5.52</v>
+      </c>
+      <c r="E13" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="F13" s="4"/>
+      <c r="G13" s="6"/>
+      <c r="H13"/>
+      <c r="I13"/>
+      <c r="J13" s="3"/>
+      <c r="K13" s="7"/>
+      <c r="L13" s="8">
+        <v>73.8</v>
+      </c>
+      <c r="M13" s="9"/>
+      <c r="N13" s="9"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="1">
+        <v>4.8600000000000003</v>
+      </c>
+      <c r="E14" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="F14" s="10"/>
+      <c r="G14"/>
+      <c r="H14"/>
+      <c r="I14"/>
+      <c r="J14" s="3"/>
+      <c r="K14" s="7"/>
+      <c r="L14" s="8">
+        <v>84.375000000000014</v>
+      </c>
+      <c r="M14" s="9"/>
+      <c r="N14" s="9"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>25</v>
+      </c>
+      <c r="D15" s="1">
+        <f>0.0002</f>
+        <v>2.0000000000000001E-4</v>
+      </c>
+      <c r="L15" s="1">
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>